<commit_message>
Proyecto 2 redes avance
</commit_message>
<xml_diff>
--- a/Proyecto Redes 1/Tablas Proyecto Redes.xlsx
+++ b/Proyecto Redes 1/Tablas Proyecto Redes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/916453d256f63eb8/Documentos/GitHub/CursosRedes/Proyecto Redes 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1006" documentId="13_ncr:1_{85A89D90-A568-47A9-B981-68FC4BAE12AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C9171B9-A204-43B2-BCD1-C85346F77B9D}"/>
+  <xr:revisionPtr revIDLastSave="1007" documentId="13_ncr:1_{85A89D90-A568-47A9-B981-68FC4BAE12AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B4D3B79-4609-4365-B80F-36071AA9B6C1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Horarios y trafico" sheetId="2" r:id="rId1"/>
@@ -1286,6 +1286,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1710,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2043,7 +2047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C95485D-07DB-4A9E-A980-AE35A914C2C8}">
   <dimension ref="B2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -2492,7 +2496,7 @@
         <v>252</v>
       </c>
       <c r="E26">
-        <f t="shared" ref="E24:E30" si="1">C26-2</f>
+        <f t="shared" ref="E26:E30" si="1">C26-2</f>
         <v>2</v>
       </c>
     </row>

</xml_diff>